<commit_message>
Small updates and added imputation.R
</commit_message>
<xml_diff>
--- a/data/scorecard/columns-simplified.xlsx
+++ b/data/scorecard/columns-simplified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbos1\Desktop\gatech\CSE6242\Project\CSE6242\data\scorecard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA94A83-9478-480E-9535-C66AB493A455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F810C959-2068-49C0-98C0-AE6776F5B1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14000" yWindow="0" windowWidth="24400" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="columns-simplified" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="339">
   <si>
     <t>NAME OF DATA ELEMENT</t>
   </si>
@@ -1033,6 +1033,21 @@
   </si>
   <si>
     <t>FINAID5</t>
+  </si>
+  <si>
+    <t>Final Name</t>
+  </si>
+  <si>
+    <t>GPA_BOTTOM_TEN_PERCENT</t>
+  </si>
+  <si>
+    <t>GPA score for the 10th percentile of admitted students</t>
+  </si>
+  <si>
+    <t>Koppen climate classification</t>
+  </si>
+  <si>
+    <t>CLIMATE_ZONE</t>
   </si>
 </sst>
 </file>
@@ -1594,16 +1609,60 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="18">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1755,62 +1814,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1825,21 +1828,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H149" totalsRowShown="0">
-  <autoFilter ref="A1:H149" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I151" totalsRowShown="0">
+  <autoFilter ref="A1:I151" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="2">
       <filters>
         <filter val="Y"/>
       </filters>
     </filterColumn>
+    <filterColumn colId="3">
+      <filters blank="1">
+        <filter val="0.418285"/>
+        <filter val="11.83149089"/>
+        <filter val="11.87630714"/>
+        <filter val="12.23483717"/>
+        <filter val="13.45981476"/>
+        <filter val="16.686585"/>
+        <filter val="17.10487003"/>
+        <filter val="18.16552136"/>
+        <filter val="20.58559904"/>
+        <filter val="20.67523155"/>
+        <filter val="21.04870033"/>
+        <filter val="21.70600538"/>
+        <filter val="22.16910666"/>
+        <filter val="4.616074096"/>
+        <filter val="41.12638183"/>
+        <filter val="46.6686585"/>
+        <filter val="66.01434"/>
+        <filter val="7.544069316"/>
+        <filter val="7.588885569"/>
+        <filter val="70.047804"/>
+        <filter val="70.30176277"/>
+        <filter val="80.90827607"/>
+        <filter val="81.2966836"/>
+        <filter val="81.80460114"/>
+        <filter val="82.52166119"/>
+        <filter val="86.49536899"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
-  <tableColumns count="8">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NAME OF DATA ELEMENT"/>
-    <tableColumn id="5" xr3:uid="{1A62A857-55EE-4685-9BD8-D21D5B302927}" name="Preprocessing Input?" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{1047D8C1-3D34-4B07-B56B-209C926DEFFA}" name="Preprocessing Output?" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{1A62A857-55EE-4685-9BD8-D21D5B302927}" name="Preprocessing Input?" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{1047D8C1-3D34-4B07-B56B-209C926DEFFA}" name="Preprocessing Output?" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Percent Missing"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="dev-category"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="VARIABLE NAME"/>
+    <tableColumn id="6" xr3:uid="{DEC2FEF7-CB61-4381-AE11-576F3919B800}" name="Final Name" dataDxfId="0"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="SOURCE"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="NOTES"/>
   </tableColumns>
@@ -2144,10 +2178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M150"/>
+  <dimension ref="A1:N151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="F145" sqref="F145"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="F151" sqref="F151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2157,12 +2191,12 @@
     <col min="3" max="3" width="22.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="13.6328125" customWidth="1"/>
-    <col min="6" max="6" width="19.36328125" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" customWidth="1"/>
-    <col min="8" max="8" width="255.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19.36328125" customWidth="1"/>
+    <col min="8" max="8" width="9.54296875" customWidth="1"/>
+    <col min="9" max="9" width="255.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2182,13 +2216,16 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
+        <v>334</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2207,11 +2244,11 @@
       <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2230,11 +2267,11 @@
       <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2253,11 +2290,11 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2276,11 +2313,11 @@
       <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2299,11 +2336,11 @@
       <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>280</v>
       </c>
@@ -2322,11 +2359,11 @@
       <c r="F7" t="s">
         <v>281</v>
       </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2345,11 +2382,11 @@
       <c r="F8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -2368,11 +2405,11 @@
       <c r="F9" t="s">
         <v>22</v>
       </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="87" hidden="1" x14ac:dyDescent="0.35">
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -2391,11 +2428,11 @@
       <c r="F10" t="s">
         <v>24</v>
       </c>
-      <c r="G10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="87" hidden="1" x14ac:dyDescent="0.35">
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -2414,11 +2451,11 @@
       <c r="F11" t="s">
         <v>26</v>
       </c>
-      <c r="G11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -2437,11 +2474,11 @@
       <c r="F12" t="s">
         <v>28</v>
       </c>
-      <c r="G12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -2460,11 +2497,11 @@
       <c r="F13" t="s">
         <v>30</v>
       </c>
-      <c r="G13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2483,11 +2520,11 @@
       <c r="F14" t="s">
         <v>32</v>
       </c>
-      <c r="G14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2506,11 +2543,11 @@
       <c r="F15" t="s">
         <v>34</v>
       </c>
-      <c r="G15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -2529,11 +2566,11 @@
       <c r="F16" t="s">
         <v>36</v>
       </c>
-      <c r="G16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -2552,11 +2589,11 @@
       <c r="F17" t="s">
         <v>38</v>
       </c>
-      <c r="G17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -2575,11 +2612,11 @@
       <c r="F18" t="s">
         <v>40</v>
       </c>
-      <c r="G18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -2598,11 +2635,11 @@
       <c r="F19" t="s">
         <v>42</v>
       </c>
-      <c r="G19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -2621,11 +2658,11 @@
       <c r="F20" t="s">
         <v>44</v>
       </c>
-      <c r="G20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -2644,11 +2681,11 @@
       <c r="F21" t="s">
         <v>46</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -2667,11 +2704,11 @@
       <c r="F22" t="s">
         <v>49</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -2690,11 +2727,11 @@
       <c r="F23" t="s">
         <v>51</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -2713,11 +2750,11 @@
       <c r="F24" t="s">
         <v>53</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -2736,11 +2773,11 @@
       <c r="F25" t="s">
         <v>55</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -2759,11 +2796,11 @@
       <c r="F26" t="s">
         <v>57</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -2782,11 +2819,11 @@
       <c r="F27" t="s">
         <v>59</v>
       </c>
-      <c r="G27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -2805,11 +2842,11 @@
       <c r="F28" t="s">
         <v>61</v>
       </c>
-      <c r="G28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -2828,11 +2865,11 @@
       <c r="F29" t="s">
         <v>63</v>
       </c>
-      <c r="G29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -2851,11 +2888,11 @@
       <c r="F30" t="s">
         <v>66</v>
       </c>
-      <c r="G30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="H30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -2874,11 +2911,11 @@
       <c r="F31" t="s">
         <v>68</v>
       </c>
-      <c r="G31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -2897,11 +2934,11 @@
       <c r="F32" t="s">
         <v>70</v>
       </c>
-      <c r="G32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -2920,11 +2957,11 @@
       <c r="F33" t="s">
         <v>72</v>
       </c>
-      <c r="G33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -2943,11 +2980,11 @@
       <c r="F34" t="s">
         <v>74</v>
       </c>
-      <c r="G34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>75</v>
       </c>
@@ -2966,11 +3003,11 @@
       <c r="F35" t="s">
         <v>76</v>
       </c>
-      <c r="G35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -2989,11 +3026,11 @@
       <c r="F36" t="s">
         <v>78</v>
       </c>
-      <c r="G36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>79</v>
       </c>
@@ -3012,11 +3049,11 @@
       <c r="F37" t="s">
         <v>80</v>
       </c>
-      <c r="G37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>81</v>
       </c>
@@ -3035,11 +3072,11 @@
       <c r="F38" t="s">
         <v>82</v>
       </c>
-      <c r="G38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -3058,11 +3095,11 @@
       <c r="F39" t="s">
         <v>84</v>
       </c>
-      <c r="G39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -3081,11 +3118,11 @@
       <c r="F40" t="s">
         <v>86</v>
       </c>
-      <c r="G40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>87</v>
       </c>
@@ -3104,11 +3141,11 @@
       <c r="F41" t="s">
         <v>88</v>
       </c>
-      <c r="G41" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>89</v>
       </c>
@@ -3127,11 +3164,11 @@
       <c r="F42" t="s">
         <v>90</v>
       </c>
-      <c r="G42" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>91</v>
       </c>
@@ -3150,11 +3187,11 @@
       <c r="F43" t="s">
         <v>92</v>
       </c>
-      <c r="G43" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>93</v>
       </c>
@@ -3173,11 +3210,11 @@
       <c r="F44" t="s">
         <v>94</v>
       </c>
-      <c r="G44" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>95</v>
       </c>
@@ -3196,11 +3233,11 @@
       <c r="F45" t="s">
         <v>96</v>
       </c>
-      <c r="G45" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -3219,11 +3256,11 @@
       <c r="F46" t="s">
         <v>98</v>
       </c>
-      <c r="G46" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>99</v>
       </c>
@@ -3242,11 +3279,11 @@
       <c r="F47" t="s">
         <v>100</v>
       </c>
-      <c r="G47" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="H47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>101</v>
       </c>
@@ -3265,11 +3302,11 @@
       <c r="F48" t="s">
         <v>102</v>
       </c>
-      <c r="G48" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>103</v>
       </c>
@@ -3288,14 +3325,14 @@
       <c r="F49" t="s">
         <v>105</v>
       </c>
-      <c r="G49" t="s">
-        <v>8</v>
-      </c>
       <c r="H49" t="s">
+        <v>8</v>
+      </c>
+      <c r="I49" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>107</v>
       </c>
@@ -3314,14 +3351,14 @@
       <c r="F50" t="s">
         <v>108</v>
       </c>
-      <c r="G50" t="s">
-        <v>8</v>
-      </c>
       <c r="H50" t="s">
+        <v>8</v>
+      </c>
+      <c r="I50" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>109</v>
       </c>
@@ -3340,14 +3377,14 @@
       <c r="F51" t="s">
         <v>110</v>
       </c>
-      <c r="G51" t="s">
-        <v>8</v>
-      </c>
       <c r="H51" t="s">
+        <v>8</v>
+      </c>
+      <c r="I51" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>111</v>
       </c>
@@ -3366,14 +3403,14 @@
       <c r="F52" t="s">
         <v>112</v>
       </c>
-      <c r="G52" t="s">
-        <v>8</v>
-      </c>
       <c r="H52" t="s">
+        <v>8</v>
+      </c>
+      <c r="I52" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>113</v>
       </c>
@@ -3392,14 +3429,14 @@
       <c r="F53" t="s">
         <v>114</v>
       </c>
-      <c r="G53" t="s">
-        <v>8</v>
-      </c>
       <c r="H53" t="s">
+        <v>8</v>
+      </c>
+      <c r="I53" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>115</v>
       </c>
@@ -3418,14 +3455,14 @@
       <c r="F54" t="s">
         <v>116</v>
       </c>
-      <c r="G54" t="s">
-        <v>8</v>
-      </c>
       <c r="H54" t="s">
+        <v>8</v>
+      </c>
+      <c r="I54" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>117</v>
       </c>
@@ -3444,14 +3481,14 @@
       <c r="F55" t="s">
         <v>118</v>
       </c>
-      <c r="G55" t="s">
-        <v>8</v>
-      </c>
       <c r="H55" t="s">
+        <v>8</v>
+      </c>
+      <c r="I55" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>119</v>
       </c>
@@ -3470,14 +3507,14 @@
       <c r="F56" t="s">
         <v>120</v>
       </c>
-      <c r="G56" t="s">
-        <v>8</v>
-      </c>
       <c r="H56" t="s">
+        <v>8</v>
+      </c>
+      <c r="I56" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>121</v>
       </c>
@@ -3496,14 +3533,14 @@
       <c r="F57" t="s">
         <v>122</v>
       </c>
-      <c r="G57" t="s">
-        <v>8</v>
-      </c>
       <c r="H57" t="s">
+        <v>8</v>
+      </c>
+      <c r="I57" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>123</v>
       </c>
@@ -3522,14 +3559,14 @@
       <c r="F58" t="s">
         <v>124</v>
       </c>
-      <c r="G58" t="s">
-        <v>8</v>
-      </c>
       <c r="H58" t="s">
+        <v>8</v>
+      </c>
+      <c r="I58" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>125</v>
       </c>
@@ -3548,14 +3585,14 @@
       <c r="F59" t="s">
         <v>126</v>
       </c>
-      <c r="G59" t="s">
-        <v>8</v>
-      </c>
       <c r="H59" t="s">
+        <v>8</v>
+      </c>
+      <c r="I59" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>127</v>
       </c>
@@ -3574,14 +3611,14 @@
       <c r="F60" t="s">
         <v>128</v>
       </c>
-      <c r="G60" t="s">
-        <v>8</v>
-      </c>
       <c r="H60" t="s">
+        <v>8</v>
+      </c>
+      <c r="I60" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>129</v>
       </c>
@@ -3600,14 +3637,14 @@
       <c r="F61" t="s">
         <v>130</v>
       </c>
-      <c r="G61" t="s">
-        <v>8</v>
-      </c>
       <c r="H61" t="s">
+        <v>8</v>
+      </c>
+      <c r="I61" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -3626,14 +3663,14 @@
       <c r="F62" t="s">
         <v>132</v>
       </c>
-      <c r="G62" t="s">
-        <v>8</v>
-      </c>
       <c r="H62" t="s">
+        <v>8</v>
+      </c>
+      <c r="I62" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>133</v>
       </c>
@@ -3652,14 +3689,14 @@
       <c r="F63" t="s">
         <v>134</v>
       </c>
-      <c r="G63" t="s">
-        <v>8</v>
-      </c>
       <c r="H63" t="s">
+        <v>8</v>
+      </c>
+      <c r="I63" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>135</v>
       </c>
@@ -3678,14 +3715,14 @@
       <c r="F64" t="s">
         <v>136</v>
       </c>
-      <c r="G64" t="s">
-        <v>8</v>
-      </c>
       <c r="H64" t="s">
+        <v>8</v>
+      </c>
+      <c r="I64" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>137</v>
       </c>
@@ -3704,14 +3741,14 @@
       <c r="F65" t="s">
         <v>138</v>
       </c>
-      <c r="G65" t="s">
-        <v>8</v>
-      </c>
       <c r="H65" t="s">
+        <v>8</v>
+      </c>
+      <c r="I65" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>139</v>
       </c>
@@ -3730,14 +3767,14 @@
       <c r="F66" t="s">
         <v>140</v>
       </c>
-      <c r="G66" t="s">
-        <v>8</v>
-      </c>
       <c r="H66" t="s">
+        <v>8</v>
+      </c>
+      <c r="I66" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>141</v>
       </c>
@@ -3756,14 +3793,14 @@
       <c r="F67" t="s">
         <v>142</v>
       </c>
-      <c r="G67" t="s">
-        <v>8</v>
-      </c>
       <c r="H67" t="s">
+        <v>8</v>
+      </c>
+      <c r="I67" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>143</v>
       </c>
@@ -3782,14 +3819,14 @@
       <c r="F68" t="s">
         <v>144</v>
       </c>
-      <c r="G68" t="s">
-        <v>8</v>
-      </c>
       <c r="H68" t="s">
+        <v>8</v>
+      </c>
+      <c r="I68" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>145</v>
       </c>
@@ -3808,14 +3845,14 @@
       <c r="F69" t="s">
         <v>146</v>
       </c>
-      <c r="G69" t="s">
-        <v>8</v>
-      </c>
       <c r="H69" t="s">
+        <v>8</v>
+      </c>
+      <c r="I69" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>147</v>
       </c>
@@ -3834,14 +3871,14 @@
       <c r="F70" t="s">
         <v>148</v>
       </c>
-      <c r="G70" t="s">
-        <v>8</v>
-      </c>
       <c r="H70" t="s">
+        <v>8</v>
+      </c>
+      <c r="I70" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>149</v>
       </c>
@@ -3860,14 +3897,14 @@
       <c r="F71" t="s">
         <v>150</v>
       </c>
-      <c r="G71" t="s">
-        <v>8</v>
-      </c>
       <c r="H71" t="s">
+        <v>8</v>
+      </c>
+      <c r="I71" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>151</v>
       </c>
@@ -3886,14 +3923,14 @@
       <c r="F72" t="s">
         <v>152</v>
       </c>
-      <c r="G72" t="s">
-        <v>8</v>
-      </c>
       <c r="H72" t="s">
+        <v>8</v>
+      </c>
+      <c r="I72" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>153</v>
       </c>
@@ -3912,14 +3949,14 @@
       <c r="F73" t="s">
         <v>154</v>
       </c>
-      <c r="G73" t="s">
-        <v>8</v>
-      </c>
       <c r="H73" t="s">
+        <v>8</v>
+      </c>
+      <c r="I73" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>155</v>
       </c>
@@ -3938,14 +3975,14 @@
       <c r="F74" t="s">
         <v>156</v>
       </c>
-      <c r="G74" t="s">
-        <v>8</v>
-      </c>
       <c r="H74" t="s">
+        <v>8</v>
+      </c>
+      <c r="I74" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>157</v>
       </c>
@@ -3964,14 +4001,14 @@
       <c r="F75" t="s">
         <v>158</v>
       </c>
-      <c r="G75" t="s">
-        <v>8</v>
-      </c>
       <c r="H75" t="s">
+        <v>8</v>
+      </c>
+      <c r="I75" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>159</v>
       </c>
@@ -3990,14 +4027,14 @@
       <c r="F76" t="s">
         <v>160</v>
       </c>
-      <c r="G76" t="s">
-        <v>8</v>
-      </c>
       <c r="H76" t="s">
+        <v>8</v>
+      </c>
+      <c r="I76" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>161</v>
       </c>
@@ -4016,14 +4053,14 @@
       <c r="F77" t="s">
         <v>162</v>
       </c>
-      <c r="G77" t="s">
-        <v>8</v>
-      </c>
       <c r="H77" t="s">
+        <v>8</v>
+      </c>
+      <c r="I77" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>163</v>
       </c>
@@ -4042,14 +4079,14 @@
       <c r="F78" t="s">
         <v>164</v>
       </c>
-      <c r="G78" t="s">
-        <v>8</v>
-      </c>
       <c r="H78" t="s">
+        <v>8</v>
+      </c>
+      <c r="I78" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>165</v>
       </c>
@@ -4068,14 +4105,14 @@
       <c r="F79" t="s">
         <v>166</v>
       </c>
-      <c r="G79" t="s">
-        <v>8</v>
-      </c>
       <c r="H79" t="s">
+        <v>8</v>
+      </c>
+      <c r="I79" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>167</v>
       </c>
@@ -4094,14 +4131,14 @@
       <c r="F80" t="s">
         <v>168</v>
       </c>
-      <c r="G80" t="s">
-        <v>8</v>
-      </c>
       <c r="H80" t="s">
+        <v>8</v>
+      </c>
+      <c r="I80" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>169</v>
       </c>
@@ -4120,14 +4157,14 @@
       <c r="F81" t="s">
         <v>170</v>
       </c>
-      <c r="G81" t="s">
-        <v>8</v>
-      </c>
       <c r="H81" t="s">
+        <v>8</v>
+      </c>
+      <c r="I81" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>171</v>
       </c>
@@ -4146,14 +4183,14 @@
       <c r="F82" t="s">
         <v>172</v>
       </c>
-      <c r="G82" t="s">
-        <v>8</v>
-      </c>
       <c r="H82" t="s">
+        <v>8</v>
+      </c>
+      <c r="I82" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>173</v>
       </c>
@@ -4172,14 +4209,14 @@
       <c r="F83" t="s">
         <v>174</v>
       </c>
-      <c r="G83" t="s">
-        <v>8</v>
-      </c>
       <c r="H83" t="s">
+        <v>8</v>
+      </c>
+      <c r="I83" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>175</v>
       </c>
@@ -4198,14 +4235,14 @@
       <c r="F84" t="s">
         <v>176</v>
       </c>
-      <c r="G84" t="s">
-        <v>8</v>
-      </c>
       <c r="H84" t="s">
+        <v>8</v>
+      </c>
+      <c r="I84" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>177</v>
       </c>
@@ -4224,14 +4261,14 @@
       <c r="F85" t="s">
         <v>178</v>
       </c>
-      <c r="G85" t="s">
-        <v>8</v>
-      </c>
       <c r="H85" t="s">
+        <v>8</v>
+      </c>
+      <c r="I85" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>179</v>
       </c>
@@ -4250,14 +4287,14 @@
       <c r="F86" t="s">
         <v>180</v>
       </c>
-      <c r="G86" t="s">
-        <v>8</v>
-      </c>
       <c r="H86" t="s">
+        <v>8</v>
+      </c>
+      <c r="I86" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>181</v>
       </c>
@@ -4276,11 +4313,11 @@
       <c r="F87" t="s">
         <v>182</v>
       </c>
-      <c r="G87" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H87" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>183</v>
       </c>
@@ -4299,14 +4336,14 @@
       <c r="F88" t="s">
         <v>185</v>
       </c>
-      <c r="G88" t="s">
-        <v>8</v>
-      </c>
       <c r="H88" t="s">
+        <v>8</v>
+      </c>
+      <c r="I88" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>187</v>
       </c>
@@ -4325,14 +4362,14 @@
       <c r="F89" t="s">
         <v>188</v>
       </c>
-      <c r="G89" t="s">
-        <v>8</v>
-      </c>
       <c r="H89" t="s">
+        <v>8</v>
+      </c>
+      <c r="I89" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>190</v>
       </c>
@@ -4351,14 +4388,14 @@
       <c r="F90" t="s">
         <v>191</v>
       </c>
-      <c r="G90" t="s">
-        <v>8</v>
-      </c>
       <c r="H90" t="s">
+        <v>8</v>
+      </c>
+      <c r="I90" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>192</v>
       </c>
@@ -4377,14 +4414,14 @@
       <c r="F91" t="s">
         <v>193</v>
       </c>
-      <c r="G91" t="s">
-        <v>8</v>
-      </c>
       <c r="H91" t="s">
+        <v>8</v>
+      </c>
+      <c r="I91" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>194</v>
       </c>
@@ -4403,14 +4440,14 @@
       <c r="F92" t="s">
         <v>195</v>
       </c>
-      <c r="G92" t="s">
-        <v>8</v>
-      </c>
       <c r="H92" t="s">
+        <v>8</v>
+      </c>
+      <c r="I92" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>196</v>
       </c>
@@ -4429,14 +4466,14 @@
       <c r="F93" t="s">
         <v>197</v>
       </c>
-      <c r="G93" t="s">
-        <v>8</v>
-      </c>
       <c r="H93" t="s">
+        <v>8</v>
+      </c>
+      <c r="I93" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>198</v>
       </c>
@@ -4455,14 +4492,14 @@
       <c r="F94" t="s">
         <v>199</v>
       </c>
-      <c r="G94" t="s">
-        <v>8</v>
-      </c>
       <c r="H94" t="s">
+        <v>8</v>
+      </c>
+      <c r="I94" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>200</v>
       </c>
@@ -4481,14 +4518,14 @@
       <c r="F95" t="s">
         <v>201</v>
       </c>
-      <c r="G95" t="s">
-        <v>8</v>
-      </c>
       <c r="H95" t="s">
+        <v>8</v>
+      </c>
+      <c r="I95" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>202</v>
       </c>
@@ -4507,14 +4544,14 @@
       <c r="F96" t="s">
         <v>203</v>
       </c>
-      <c r="G96" t="s">
-        <v>8</v>
-      </c>
       <c r="H96" t="s">
+        <v>8</v>
+      </c>
+      <c r="I96" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>204</v>
       </c>
@@ -4533,14 +4570,14 @@
       <c r="F97" t="s">
         <v>205</v>
       </c>
-      <c r="G97" t="s">
-        <v>8</v>
-      </c>
       <c r="H97" t="s">
+        <v>8</v>
+      </c>
+      <c r="I97" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>206</v>
       </c>
@@ -4559,11 +4596,11 @@
       <c r="F98" t="s">
         <v>207</v>
       </c>
-      <c r="G98" t="s">
+      <c r="H98" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>208</v>
       </c>
@@ -4582,14 +4619,14 @@
       <c r="F99" t="s">
         <v>210</v>
       </c>
-      <c r="G99" t="s">
-        <v>8</v>
-      </c>
       <c r="H99" t="s">
+        <v>8</v>
+      </c>
+      <c r="I99" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>212</v>
       </c>
@@ -4608,14 +4645,14 @@
       <c r="F100" t="s">
         <v>213</v>
       </c>
-      <c r="G100" t="s">
-        <v>8</v>
-      </c>
       <c r="H100" t="s">
+        <v>8</v>
+      </c>
+      <c r="I100" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>214</v>
       </c>
@@ -4634,11 +4671,11 @@
       <c r="F101" t="s">
         <v>215</v>
       </c>
-      <c r="G101" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="H101" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>216</v>
       </c>
@@ -4657,11 +4694,11 @@
       <c r="F102" t="s">
         <v>217</v>
       </c>
-      <c r="G102" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="H102" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>218</v>
       </c>
@@ -4680,14 +4717,14 @@
       <c r="F103" t="s">
         <v>219</v>
       </c>
-      <c r="G103" t="s">
-        <v>8</v>
-      </c>
       <c r="H103" t="s">
+        <v>8</v>
+      </c>
+      <c r="I103" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>221</v>
       </c>
@@ -4706,14 +4743,14 @@
       <c r="F104" t="s">
         <v>222</v>
       </c>
-      <c r="G104" t="s">
-        <v>8</v>
-      </c>
       <c r="H104" t="s">
+        <v>8</v>
+      </c>
+      <c r="I104" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>224</v>
       </c>
@@ -4732,14 +4769,14 @@
       <c r="F105" t="s">
         <v>225</v>
       </c>
-      <c r="G105" t="s">
-        <v>8</v>
-      </c>
       <c r="H105" t="s">
+        <v>8</v>
+      </c>
+      <c r="I105" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>227</v>
       </c>
@@ -4758,14 +4795,14 @@
       <c r="F106" t="s">
         <v>228</v>
       </c>
-      <c r="G106" t="s">
-        <v>8</v>
-      </c>
       <c r="H106" t="s">
+        <v>8</v>
+      </c>
+      <c r="I106" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>230</v>
       </c>
@@ -4784,14 +4821,14 @@
       <c r="F107" t="s">
         <v>231</v>
       </c>
-      <c r="G107" t="s">
-        <v>8</v>
-      </c>
       <c r="H107" t="s">
+        <v>8</v>
+      </c>
+      <c r="I107" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>233</v>
       </c>
@@ -4810,11 +4847,11 @@
       <c r="F108" t="s">
         <v>235</v>
       </c>
-      <c r="G108" t="s">
+      <c r="H108" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>237</v>
       </c>
@@ -4833,11 +4870,11 @@
       <c r="F109" t="s">
         <v>238</v>
       </c>
-      <c r="G109" t="s">
+      <c r="H109" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>239</v>
       </c>
@@ -4856,11 +4893,11 @@
       <c r="F110" t="s">
         <v>240</v>
       </c>
-      <c r="G110" t="s">
+      <c r="H110" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>241</v>
       </c>
@@ -4879,11 +4916,11 @@
       <c r="F111" t="s">
         <v>242</v>
       </c>
-      <c r="G111" t="s">
+      <c r="H111" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>243</v>
       </c>
@@ -4902,11 +4939,11 @@
       <c r="F112" t="s">
         <v>244</v>
       </c>
-      <c r="G112" t="s">
+      <c r="H112" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>245</v>
       </c>
@@ -4925,11 +4962,11 @@
       <c r="F113" t="s">
         <v>246</v>
       </c>
-      <c r="G113" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H113" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>247</v>
       </c>
@@ -4948,11 +4985,11 @@
       <c r="F114" t="s">
         <v>248</v>
       </c>
-      <c r="G114" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="H114" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>249</v>
       </c>
@@ -4971,11 +5008,11 @@
       <c r="F115" t="s">
         <v>250</v>
       </c>
-      <c r="G115" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H115" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>251</v>
       </c>
@@ -4994,11 +5031,11 @@
       <c r="F116" t="s">
         <v>252</v>
       </c>
-      <c r="G116" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H116" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>253</v>
       </c>
@@ -5017,11 +5054,11 @@
       <c r="F117" t="s">
         <v>254</v>
       </c>
-      <c r="G117" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H117" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>257</v>
       </c>
@@ -5040,11 +5077,11 @@
       <c r="F118" t="s">
         <v>258</v>
       </c>
-      <c r="G118" t="s">
+      <c r="H118" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>259</v>
       </c>
@@ -5063,11 +5100,11 @@
       <c r="F119" t="s">
         <v>260</v>
       </c>
-      <c r="G119" t="s">
+      <c r="H119" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>261</v>
       </c>
@@ -5086,11 +5123,11 @@
       <c r="F120" t="s">
         <v>262</v>
       </c>
-      <c r="G120" t="s">
+      <c r="H120" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>263</v>
       </c>
@@ -5109,11 +5146,11 @@
       <c r="F121" t="s">
         <v>264</v>
       </c>
-      <c r="G121" t="s">
+      <c r="H121" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>265</v>
       </c>
@@ -5132,11 +5169,11 @@
       <c r="F122" t="s">
         <v>266</v>
       </c>
-      <c r="G122" t="s">
+      <c r="H122" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
         <v>268</v>
       </c>
@@ -5155,11 +5192,12 @@
       <c r="F123" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="G123" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G123" s="3"/>
+      <c r="H123" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
         <v>270</v>
       </c>
@@ -5178,11 +5216,12 @@
       <c r="F124" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="G124" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G124" s="3"/>
+      <c r="H124" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>272</v>
       </c>
@@ -5201,11 +5240,12 @@
       <c r="F125" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="G125" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G125" s="3"/>
+      <c r="H125" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
         <v>274</v>
       </c>
@@ -5224,11 +5264,12 @@
       <c r="F126" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="G126" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G126" s="3"/>
+      <c r="H126" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>276</v>
       </c>
@@ -5247,11 +5288,12 @@
       <c r="F127" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G127" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G127" s="3"/>
+      <c r="H127" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="s">
         <v>282</v>
       </c>
@@ -5270,14 +5312,15 @@
       <c r="F128" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="G128" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="G128" s="4"/>
       <c r="H128" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I128" s="4" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
         <v>285</v>
       </c>
@@ -5296,14 +5339,15 @@
       <c r="F129" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="G129" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="G129" s="4"/>
       <c r="H129" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I129" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="s">
         <v>287</v>
       </c>
@@ -5322,14 +5366,15 @@
       <c r="F130" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="G130" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="G130" s="4"/>
       <c r="H130" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I130" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" s="4" t="s">
         <v>289</v>
       </c>
@@ -5348,14 +5393,15 @@
       <c r="F131" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="G131" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="G131" s="4"/>
       <c r="H131" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I131" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="132" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" s="4" t="s">
         <v>291</v>
       </c>
@@ -5374,14 +5420,15 @@
       <c r="F132" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="G132" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="G132" s="4"/>
       <c r="H132" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I132" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="s">
         <v>293</v>
       </c>
@@ -5400,14 +5447,15 @@
       <c r="F133" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="G133" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="G133" s="4"/>
       <c r="H133" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I133" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="134" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="s">
         <v>295</v>
       </c>
@@ -5426,14 +5474,15 @@
       <c r="F134" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="G134" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="G134" s="4"/>
       <c r="H134" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I134" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="s">
         <v>297</v>
       </c>
@@ -5452,14 +5501,15 @@
       <c r="F135" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="G135" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="G135" s="4"/>
       <c r="H135" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I135" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="136" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="s">
         <v>299</v>
       </c>
@@ -5478,14 +5528,15 @@
       <c r="F136" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="G136" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="G136" s="4"/>
       <c r="H136" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I136" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="137" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="s">
         <v>301</v>
       </c>
@@ -5504,14 +5555,15 @@
       <c r="F137" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="G137" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="G137" s="4"/>
       <c r="H137" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I137" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="s">
         <v>303</v>
       </c>
@@ -5530,14 +5582,15 @@
       <c r="F138" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="G138" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="G138" s="4"/>
       <c r="H138" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I138" s="4" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="139" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" s="4" t="s">
         <v>306</v>
       </c>
@@ -5556,14 +5609,15 @@
       <c r="F139" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="G139" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="G139" s="4"/>
       <c r="H139" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I139" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A140" s="4" t="s">
         <v>308</v>
       </c>
@@ -5582,14 +5636,15 @@
       <c r="F140" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="G140" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="G140" s="4"/>
       <c r="H140" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I140" s="4" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>315</v>
       </c>
@@ -5605,16 +5660,16 @@
       <c r="F141" t="s">
         <v>316</v>
       </c>
-      <c r="H141" t="s">
+      <c r="I141" t="s">
         <v>317</v>
       </c>
-      <c r="I141" s="4"/>
       <c r="J141" s="4"/>
       <c r="K141" s="4"/>
       <c r="L141" s="4"/>
       <c r="M141" s="4"/>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N141" s="4"/>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>318</v>
       </c>
@@ -5630,16 +5685,16 @@
       <c r="F142" t="s">
         <v>319</v>
       </c>
-      <c r="H142" t="s">
+      <c r="I142" t="s">
         <v>317</v>
       </c>
-      <c r="I142" s="4"/>
       <c r="J142" s="4"/>
       <c r="K142" s="4"/>
       <c r="L142" s="4"/>
       <c r="M142" s="4"/>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N142" s="4"/>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>320</v>
       </c>
@@ -5655,16 +5710,16 @@
       <c r="F143" t="s">
         <v>321</v>
       </c>
-      <c r="H143" t="s">
+      <c r="I143" t="s">
         <v>317</v>
       </c>
-      <c r="I143" s="4"/>
       <c r="J143" s="4"/>
       <c r="K143" s="4"/>
       <c r="L143" s="4"/>
       <c r="M143" s="4"/>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N143" s="4"/>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>322</v>
       </c>
@@ -5680,16 +5735,16 @@
       <c r="F144" t="s">
         <v>323</v>
       </c>
-      <c r="H144" t="s">
+      <c r="I144" t="s">
         <v>317</v>
       </c>
-      <c r="I144" s="4"/>
       <c r="J144" s="4"/>
       <c r="K144" s="4"/>
       <c r="L144" s="4"/>
       <c r="M144" s="4"/>
-    </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N144" s="4"/>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A145" s="4" t="s">
         <v>324</v>
       </c>
@@ -5706,14 +5761,15 @@
       <c r="F145" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="H145" s="4"/>
+      <c r="G145" s="4"/>
       <c r="I145" s="4"/>
       <c r="J145" s="4"/>
       <c r="K145" s="4"/>
       <c r="L145" s="4"/>
       <c r="M145" s="4"/>
-    </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N145" s="4"/>
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A146" s="4" t="s">
         <v>325</v>
       </c>
@@ -5737,8 +5793,9 @@
       <c r="K146" s="4"/>
       <c r="L146" s="4"/>
       <c r="M146" s="4"/>
-    </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N146" s="4"/>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A147" s="4" t="s">
         <v>326</v>
       </c>
@@ -5762,8 +5819,9 @@
       <c r="K147" s="4"/>
       <c r="L147" s="4"/>
       <c r="M147" s="4"/>
-    </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N147" s="4"/>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A148" s="4" t="s">
         <v>327</v>
       </c>
@@ -5787,8 +5845,9 @@
       <c r="K148" s="4"/>
       <c r="L148" s="4"/>
       <c r="M148" s="4"/>
-    </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N148" s="4"/>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A149" s="4" t="s">
         <v>328</v>
       </c>
@@ -5812,14 +5871,25 @@
       <c r="K149" s="4"/>
       <c r="L149" s="4"/>
       <c r="M149" s="4"/>
-    </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A150" s="4"/>
-      <c r="B150" s="4"/>
-      <c r="C150" s="4"/>
+      <c r="N149" s="4"/>
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A150" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B150" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>313</v>
+      </c>
       <c r="D150" s="4"/>
-      <c r="E150" s="4"/>
-      <c r="F150" s="4"/>
+      <c r="E150" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F150" s="4" t="s">
+        <v>335</v>
+      </c>
       <c r="G150" s="4"/>
       <c r="H150" s="4"/>
       <c r="I150" s="4"/>
@@ -5827,47 +5897,66 @@
       <c r="K150" s="4"/>
       <c r="L150" s="4"/>
       <c r="M150" s="4"/>
+      <c r="N150" s="4"/>
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>337</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C151" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="E151" t="s">
+        <v>10</v>
+      </c>
+      <c r="F151" t="s">
+        <v>338</v>
+      </c>
+      <c r="G151" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="F123:F127">
+  <conditionalFormatting sqref="F123:G127">
     <cfRule type="duplicateValues" dxfId="17" priority="21"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F123:F127">
+  <conditionalFormatting sqref="F123:G127">
     <cfRule type="duplicateValues" dxfId="16" priority="22"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H146:H150">
+  <conditionalFormatting sqref="I146:I150">
     <cfRule type="duplicateValues" dxfId="15" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E146:E150">
     <cfRule type="duplicateValues" dxfId="14" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F128:F137">
+  <conditionalFormatting sqref="F128:G137">
     <cfRule type="duplicateValues" dxfId="13" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F128:F137">
+  <conditionalFormatting sqref="F128:G137">
     <cfRule type="duplicateValues" dxfId="12" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F138:F139">
+  <conditionalFormatting sqref="F138:G139">
     <cfRule type="duplicateValues" dxfId="11" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F138:F139">
+  <conditionalFormatting sqref="F138:G139">
     <cfRule type="duplicateValues" dxfId="10" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H145">
-    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
+  <conditionalFormatting sqref="I145">
+    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H145">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  <conditionalFormatting sqref="I145">
+    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145">
-    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F140">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+  <conditionalFormatting sqref="F140:G140">
+    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F140">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  <conditionalFormatting sqref="F140:G140">
+    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5973,10 +6062,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D6">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D6">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix gpa truncation and fix urls
</commit_message>
<xml_diff>
--- a/data/scorecard/columns-simplified.xlsx
+++ b/data/scorecard/columns-simplified.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbos1\Desktop\gatech\CSE6242\Project\CSE6242\data\scorecard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2196D66E-7ACB-4854-8CBD-1D6E4B61F471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFA5288-0FDD-4704-94F9-7964806FE235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2062,7 +2062,115 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2201,124 +2309,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2334,26 +2324,15 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:M220" totalsRowShown="0">
-  <autoFilter ref="A1:M220" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Y"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <filters>
-        <filter val="N"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M220" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NAME OF DATA ELEMENT"/>
-    <tableColumn id="13" xr3:uid="{06CDB540-C637-449E-A0D3-23E77B1FFF5A}" name="Type" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{1A62A857-55EE-4685-9BD8-D21D5B302927}" name="Preprocessing Input?" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{1047D8C1-3D34-4B07-B56B-209C926DEFFA}" name="Preprocessing Output?" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{7F48CE00-C0E5-4D18-8506-F5FBCB5FB7B8}" name="Used with the imputation algorithm?" dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{130CE4DF-DD3C-4EA1-941B-A785EAA02A20}" name="Checked for consistency after imputation?" dataDxfId="16"/>
-    <tableColumn id="15" xr3:uid="{688646D9-13EC-4083-AD76-A2ADE04C8F52}" name="Dummy variable source" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{06CDB540-C637-449E-A0D3-23E77B1FFF5A}" name="Type" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{1A62A857-55EE-4685-9BD8-D21D5B302927}" name="Preprocessing Input?" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{1047D8C1-3D34-4B07-B56B-209C926DEFFA}" name="Preprocessing Output?" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{7F48CE00-C0E5-4D18-8506-F5FBCB5FB7B8}" name="Used with the imputation algorithm?" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{130CE4DF-DD3C-4EA1-941B-A785EAA02A20}" name="Checked for consistency after imputation?" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{688646D9-13EC-4083-AD76-A2ADE04C8F52}" name="Dummy variable source" dataDxfId="1"/>
     <tableColumn id="16" xr3:uid="{90A754FA-5AE0-422C-94B0-BDDFA2826BA9}" name="Weight (default)" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Percent Missing"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="dev-category"/>
@@ -2665,8 +2644,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R220"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K48" sqref="K2:K220"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2724,7 +2703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2762,7 +2741,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2800,7 +2779,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2838,7 +2817,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2876,7 +2855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2914,7 +2893,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>263</v>
       </c>
@@ -2952,7 +2931,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2987,7 +2966,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -3060,7 +3039,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="87" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -3098,7 +3077,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -3133,7 +3112,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -3168,7 +3147,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -3203,7 +3182,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -3238,7 +3217,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -3387,7 +3366,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -3422,7 +3401,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -3457,7 +3436,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -3492,7 +3471,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -3527,7 +3506,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -3562,7 +3541,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -3597,7 +3576,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -3632,7 +3611,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -3667,7 +3646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -3702,7 +3681,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -3737,7 +3716,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -3810,7 +3789,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -3845,7 +3824,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -3880,7 +3859,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -3915,7 +3894,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>75</v>
       </c>
@@ -3950,7 +3929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -3985,7 +3964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>79</v>
       </c>
@@ -4020,7 +3999,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>81</v>
       </c>
@@ -4055,7 +4034,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -4090,7 +4069,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -4125,7 +4104,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>87</v>
       </c>
@@ -4160,7 +4139,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>89</v>
       </c>
@@ -4195,7 +4174,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>91</v>
       </c>
@@ -4230,7 +4209,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>93</v>
       </c>
@@ -4265,7 +4244,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>95</v>
       </c>
@@ -4300,7 +4279,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -4335,7 +4314,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>99</v>
       </c>
@@ -4408,7 +4387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>103</v>
       </c>
@@ -4446,7 +4425,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>107</v>
       </c>
@@ -4484,7 +4463,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>109</v>
       </c>
@@ -4522,7 +4501,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>111</v>
       </c>
@@ -4560,7 +4539,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>113</v>
       </c>
@@ -4598,7 +4577,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>115</v>
       </c>
@@ -4636,7 +4615,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>117</v>
       </c>
@@ -4674,7 +4653,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>119</v>
       </c>
@@ -4712,7 +4691,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>121</v>
       </c>
@@ -4750,7 +4729,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>123</v>
       </c>
@@ -4788,7 +4767,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>125</v>
       </c>
@@ -4826,7 +4805,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>127</v>
       </c>
@@ -4864,7 +4843,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>129</v>
       </c>
@@ -4902,7 +4881,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -4940,7 +4919,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>133</v>
       </c>
@@ -4978,7 +4957,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>135</v>
       </c>
@@ -5016,7 +4995,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>137</v>
       </c>
@@ -5054,7 +5033,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>139</v>
       </c>
@@ -5092,7 +5071,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>141</v>
       </c>
@@ -5130,7 +5109,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>143</v>
       </c>
@@ -5168,7 +5147,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>145</v>
       </c>
@@ -5206,7 +5185,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>147</v>
       </c>
@@ -5244,7 +5223,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>149</v>
       </c>
@@ -5282,7 +5261,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>151</v>
       </c>
@@ -5320,7 +5299,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>153</v>
       </c>
@@ -5358,7 +5337,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>155</v>
       </c>
@@ -5396,7 +5375,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>157</v>
       </c>
@@ -5434,7 +5413,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>159</v>
       </c>
@@ -5472,7 +5451,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>161</v>
       </c>
@@ -5510,7 +5489,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>163</v>
       </c>
@@ -5548,7 +5527,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>165</v>
       </c>
@@ -5586,7 +5565,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>167</v>
       </c>
@@ -5624,7 +5603,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>169</v>
       </c>
@@ -5662,7 +5641,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>171</v>
       </c>
@@ -5700,7 +5679,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>173</v>
       </c>
@@ -5738,7 +5717,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>175</v>
       </c>
@@ -5776,7 +5755,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>177</v>
       </c>
@@ -5814,7 +5793,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>179</v>
       </c>
@@ -5852,7 +5831,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>181</v>
       </c>
@@ -5887,7 +5866,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>183</v>
       </c>
@@ -5925,7 +5904,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>205</v>
       </c>
@@ -6004,7 +5983,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>211</v>
       </c>
@@ -6045,7 +6024,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>213</v>
       </c>
@@ -6080,7 +6059,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>215</v>
       </c>
@@ -6115,7 +6094,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>217</v>
       </c>
@@ -6153,7 +6132,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>220</v>
       </c>
@@ -6191,7 +6170,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>223</v>
       </c>
@@ -6229,7 +6208,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>226</v>
       </c>
@@ -6267,7 +6246,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>229</v>
       </c>
@@ -6305,7 +6284,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>234</v>
       </c>
@@ -6340,7 +6319,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>236</v>
       </c>
@@ -6375,7 +6354,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>238</v>
       </c>
@@ -6410,7 +6389,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:13" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="6" t="s">
         <v>442</v>
       </c>
@@ -6439,7 +6418,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="103" spans="1:13" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A103" s="6" t="s">
         <v>441</v>
       </c>
@@ -6468,7 +6447,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>242</v>
       </c>
@@ -6503,7 +6482,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="105" spans="1:13" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A105" s="6" t="s">
         <v>459</v>
       </c>
@@ -6532,7 +6511,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="106" spans="1:13" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A106" s="6" t="s">
         <v>461</v>
       </c>
@@ -6561,7 +6540,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="107" spans="1:13" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="6" t="s">
         <v>460</v>
       </c>
@@ -6590,7 +6569,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="108" spans="1:13" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A108" s="6" t="s">
         <v>462</v>
       </c>
@@ -6619,7 +6598,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>244</v>
       </c>
@@ -6654,7 +6633,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>246</v>
       </c>
@@ -6689,7 +6668,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A111" s="6" t="s">
         <v>250</v>
       </c>
@@ -6724,7 +6703,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>248</v>
       </c>
@@ -6759,7 +6738,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="113" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
         <v>253</v>
       </c>
@@ -6794,7 +6773,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
         <v>255</v>
       </c>
@@ -6829,7 +6808,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
         <v>257</v>
       </c>
@@ -6864,7 +6843,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
         <v>259</v>
       </c>
@@ -6899,7 +6878,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
         <v>261</v>
       </c>
@@ -6934,7 +6913,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A118" s="4" t="s">
         <v>265</v>
       </c>
@@ -6975,7 +6954,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
         <v>268</v>
       </c>
@@ -7016,7 +6995,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="120" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A120" s="4" t="s">
         <v>270</v>
       </c>
@@ -7057,7 +7036,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
         <v>272</v>
       </c>
@@ -7098,7 +7077,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="122" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
         <v>274</v>
       </c>
@@ -7139,7 +7118,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="123" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
         <v>276</v>
       </c>
@@ -7180,7 +7159,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="s">
         <v>278</v>
       </c>
@@ -7221,7 +7200,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="125" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="s">
         <v>280</v>
       </c>
@@ -7262,7 +7241,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
         <v>282</v>
       </c>
@@ -7303,7 +7282,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="127" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="s">
         <v>284</v>
       </c>
@@ -7344,7 +7323,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="s">
         <v>286</v>
       </c>
@@ -7385,7 +7364,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="129" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
         <v>289</v>
       </c>
@@ -7606,7 +7585,7 @@
       <c r="L135" s="4"/>
       <c r="M135" s="4"/>
     </row>
-    <row r="136" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="s">
         <v>291</v>
       </c>
@@ -7644,7 +7623,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="137" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>298</v>
       </c>
@@ -7681,7 +7660,7 @@
       <c r="Q137" s="4"/>
       <c r="R137" s="4"/>
     </row>
-    <row r="138" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>301</v>
       </c>
@@ -7718,7 +7697,7 @@
       <c r="Q138" s="4"/>
       <c r="R138" s="4"/>
     </row>
-    <row r="139" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>303</v>
       </c>
@@ -7755,7 +7734,7 @@
       <c r="Q139" s="4"/>
       <c r="R139" s="4"/>
     </row>
-    <row r="140" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>305</v>
       </c>
@@ -7792,7 +7771,7 @@
       <c r="Q140" s="4"/>
       <c r="R140" s="4"/>
     </row>
-    <row r="141" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="s">
         <v>307</v>
       </c>
@@ -7828,7 +7807,7 @@
       <c r="Q141" s="4"/>
       <c r="R141" s="4"/>
     </row>
-    <row r="142" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A142" s="4" t="s">
         <v>308</v>
       </c>
@@ -7865,7 +7844,7 @@
       <c r="Q142" s="4"/>
       <c r="R142" s="4"/>
     </row>
-    <row r="143" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A143" s="4" t="s">
         <v>309</v>
       </c>
@@ -7902,7 +7881,7 @@
       <c r="Q143" s="4"/>
       <c r="R143" s="4"/>
     </row>
-    <row r="144" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A144" s="4" t="s">
         <v>310</v>
       </c>
@@ -7939,7 +7918,7 @@
       <c r="Q144" s="4"/>
       <c r="R144" s="4"/>
     </row>
-    <row r="145" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A145" s="4" t="s">
         <v>311</v>
       </c>
@@ -7976,12 +7955,12 @@
       <c r="Q145" s="4"/>
       <c r="R145" s="4"/>
     </row>
-    <row r="146" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A146" s="4" t="s">
         <v>318</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C146" s="4" t="s">
         <v>296</v>
@@ -8013,7 +7992,7 @@
       <c r="Q146" s="4"/>
       <c r="R146" s="4"/>
     </row>
-    <row r="147" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>319</v>
       </c>
@@ -8042,7 +8021,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="148" spans="1:18" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A148" s="6" t="s">
         <v>478</v>
       </c>
@@ -8072,7 +8051,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="149" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A149" s="4" t="s">
         <v>187</v>
       </c>
@@ -8108,7 +8087,7 @@
       </c>
       <c r="M149" s="2"/>
     </row>
-    <row r="150" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A150" s="4" t="s">
         <v>189</v>
       </c>
@@ -8144,7 +8123,7 @@
       </c>
       <c r="M150" s="2"/>
     </row>
-    <row r="151" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A151" s="4" t="s">
         <v>191</v>
       </c>
@@ -8180,7 +8159,7 @@
       </c>
       <c r="M151" s="2"/>
     </row>
-    <row r="152" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A152" s="4" t="s">
         <v>193</v>
       </c>
@@ -8216,7 +8195,7 @@
       </c>
       <c r="M152" s="2"/>
     </row>
-    <row r="153" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A153" s="4" t="s">
         <v>195</v>
       </c>
@@ -8252,7 +8231,7 @@
       </c>
       <c r="M153" s="2"/>
     </row>
-    <row r="154" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A154" s="4" t="s">
         <v>197</v>
       </c>
@@ -8288,7 +8267,7 @@
       </c>
       <c r="M154" s="2"/>
     </row>
-    <row r="155" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A155" s="4" t="s">
         <v>199</v>
       </c>
@@ -8323,7 +8302,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="156" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A156" s="4" t="s">
         <v>201</v>
       </c>
@@ -8358,7 +8337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="157" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A157" s="4" t="s">
         <v>203</v>
       </c>
@@ -8393,7 +8372,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="158" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A158" s="4" t="s">
         <v>322</v>
       </c>
@@ -8429,7 +8408,7 @@
       </c>
       <c r="M158" s="2"/>
     </row>
-    <row r="159" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A159" s="4" t="s">
         <v>324</v>
       </c>
@@ -8465,7 +8444,7 @@
       </c>
       <c r="M159" s="2"/>
     </row>
-    <row r="160" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A160" s="4" t="s">
         <v>326</v>
       </c>
@@ -8501,7 +8480,7 @@
       </c>
       <c r="M160" s="2"/>
     </row>
-    <row r="161" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A161" s="4" t="s">
         <v>328</v>
       </c>
@@ -8537,7 +8516,7 @@
       </c>
       <c r="M161" s="2"/>
     </row>
-    <row r="162" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A162" s="4" t="s">
         <v>330</v>
       </c>
@@ -8573,7 +8552,7 @@
       </c>
       <c r="M162" s="2"/>
     </row>
-    <row r="163" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>333</v>
       </c>
@@ -8605,7 +8584,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="164" spans="1:13" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A164" s="6" t="s">
         <v>450</v>
       </c>
@@ -8631,7 +8610,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="165" spans="1:13" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A165" s="6" t="s">
         <v>336</v>
       </c>
@@ -8664,7 +8643,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="166" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A166" s="5" t="s">
         <v>335</v>
       </c>
@@ -8696,7 +8675,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="167" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A167" s="6" t="s">
         <v>339</v>
       </c>
@@ -8728,7 +8707,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="168" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A168" s="6" t="s">
         <v>340</v>
       </c>
@@ -8760,7 +8739,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="169" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A169" s="6" t="s">
         <v>341</v>
       </c>
@@ -8792,7 +8771,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="170" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>347</v>
       </c>
@@ -8824,7 +8803,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="171" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>458</v>
       </c>
@@ -8859,7 +8838,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="172" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>350</v>
       </c>
@@ -8891,7 +8870,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="173" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>353</v>
       </c>
@@ -8923,7 +8902,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="174" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>355</v>
       </c>
@@ -8955,7 +8934,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="175" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>357</v>
       </c>
@@ -8987,7 +8966,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="176" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>358</v>
       </c>
@@ -9019,7 +8998,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>359</v>
       </c>
@@ -9051,7 +9030,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>360</v>
       </c>
@@ -9083,7 +9062,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A179" s="4" t="s">
         <v>365</v>
       </c>
@@ -9116,7 +9095,7 @@
       </c>
       <c r="L179" s="4"/>
     </row>
-    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A180" s="4" t="s">
         <v>367</v>
       </c>
@@ -9149,7 +9128,7 @@
       </c>
       <c r="L180" s="4"/>
     </row>
-    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A181" s="4" t="s">
         <v>369</v>
       </c>
@@ -9182,7 +9161,7 @@
       </c>
       <c r="L181" s="4"/>
     </row>
-    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A182" s="4" t="s">
         <v>371</v>
       </c>
@@ -9215,7 +9194,7 @@
       </c>
       <c r="L182" s="4"/>
     </row>
-    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A183" s="4" t="s">
         <v>373</v>
       </c>
@@ -9248,7 +9227,7 @@
       </c>
       <c r="L183" s="4"/>
     </row>
-    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A184" s="4" t="s">
         <v>375</v>
       </c>
@@ -9281,7 +9260,7 @@
       </c>
       <c r="L184" s="4"/>
     </row>
-    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A185" s="4" t="s">
         <v>377</v>
       </c>
@@ -9314,7 +9293,7 @@
       </c>
       <c r="L185" s="4"/>
     </row>
-    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A186" s="4" t="s">
         <v>379</v>
       </c>
@@ -9347,7 +9326,7 @@
       </c>
       <c r="L186" s="4"/>
     </row>
-    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A187" s="4" t="s">
         <v>381</v>
       </c>
@@ -9380,7 +9359,7 @@
       </c>
       <c r="L187" s="4"/>
     </row>
-    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A188" s="4" t="s">
         <v>383</v>
       </c>
@@ -9413,7 +9392,7 @@
       </c>
       <c r="L188" s="6"/>
     </row>
-    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A189" s="4" t="s">
         <v>385</v>
       </c>
@@ -9446,7 +9425,7 @@
       </c>
       <c r="L189" s="6"/>
     </row>
-    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A190" s="4" t="s">
         <v>387</v>
       </c>
@@ -9479,7 +9458,7 @@
       </c>
       <c r="L190" s="6"/>
     </row>
-    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A191" s="4" t="s">
         <v>389</v>
       </c>
@@ -9512,7 +9491,7 @@
       </c>
       <c r="L191" s="6"/>
     </row>
-    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A192" s="4" t="s">
         <v>391</v>
       </c>
@@ -9545,7 +9524,7 @@
       </c>
       <c r="L192" s="6"/>
     </row>
-    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A193" s="4" t="s">
         <v>393</v>
       </c>
@@ -9578,7 +9557,7 @@
       </c>
       <c r="L193" s="6"/>
     </row>
-    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A194" s="4" t="s">
         <v>395</v>
       </c>
@@ -9611,7 +9590,7 @@
       </c>
       <c r="L194" s="6"/>
     </row>
-    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A195" s="4" t="s">
         <v>397</v>
       </c>
@@ -9644,7 +9623,7 @@
       </c>
       <c r="L195" s="6"/>
     </row>
-    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A196" s="4" t="s">
         <v>399</v>
       </c>
@@ -9677,7 +9656,7 @@
       </c>
       <c r="L196" s="6"/>
     </row>
-    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A197" s="4" t="s">
         <v>401</v>
       </c>
@@ -9710,7 +9689,7 @@
       </c>
       <c r="L197" s="6"/>
     </row>
-    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A198" s="4" t="s">
         <v>403</v>
       </c>
@@ -9743,7 +9722,7 @@
       </c>
       <c r="L198" s="6"/>
     </row>
-    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A199" s="4" t="s">
         <v>405</v>
       </c>
@@ -9776,7 +9755,7 @@
       </c>
       <c r="L199" s="6"/>
     </row>
-    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A200" s="4" t="s">
         <v>407</v>
       </c>
@@ -9809,7 +9788,7 @@
       </c>
       <c r="L200" s="6"/>
     </row>
-    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A201" s="4" t="s">
         <v>409</v>
       </c>
@@ -9842,7 +9821,7 @@
       </c>
       <c r="L201" s="6"/>
     </row>
-    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A202" s="4" t="s">
         <v>411</v>
       </c>
@@ -9875,7 +9854,7 @@
       </c>
       <c r="L202" s="6"/>
     </row>
-    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A203" s="4" t="s">
         <v>413</v>
       </c>
@@ -9908,7 +9887,7 @@
       </c>
       <c r="L203" s="6"/>
     </row>
-    <row r="204" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A204" s="4" t="s">
         <v>415</v>
       </c>
@@ -9941,7 +9920,7 @@
       </c>
       <c r="L204" s="6"/>
     </row>
-    <row r="205" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A205" s="4" t="s">
         <v>417</v>
       </c>
@@ -9974,7 +9953,7 @@
       </c>
       <c r="L205" s="6"/>
     </row>
-    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A206" s="4" t="s">
         <v>419</v>
       </c>
@@ -10007,7 +9986,7 @@
       </c>
       <c r="L206" s="6"/>
     </row>
-    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A207" s="4" t="s">
         <v>421</v>
       </c>
@@ -10040,7 +10019,7 @@
       </c>
       <c r="L207" s="6"/>
     </row>
-    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A208" s="4" t="s">
         <v>423</v>
       </c>
@@ -10073,7 +10052,7 @@
       </c>
       <c r="L208" s="6"/>
     </row>
-    <row r="209" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A209" s="4" t="s">
         <v>425</v>
       </c>
@@ -10106,7 +10085,7 @@
       </c>
       <c r="L209" s="6"/>
     </row>
-    <row r="210" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A210" s="4" t="s">
         <v>427</v>
       </c>
@@ -10139,7 +10118,7 @@
       </c>
       <c r="L210" s="6"/>
     </row>
-    <row r="211" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A211" s="4" t="s">
         <v>429</v>
       </c>
@@ -10172,7 +10151,7 @@
       </c>
       <c r="L211" s="6"/>
     </row>
-    <row r="212" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A212" s="4" t="s">
         <v>431</v>
       </c>
@@ -10205,7 +10184,7 @@
       </c>
       <c r="L212" s="6"/>
     </row>
-    <row r="213" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A213" s="4" t="s">
         <v>433</v>
       </c>
@@ -10238,7 +10217,7 @@
       </c>
       <c r="L213" s="6"/>
     </row>
-    <row r="214" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A214" s="4" t="s">
         <v>435</v>
       </c>
@@ -10271,7 +10250,7 @@
       </c>
       <c r="L214" s="6"/>
     </row>
-    <row r="215" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A215" s="4" t="s">
         <v>437</v>
       </c>
@@ -10304,7 +10283,7 @@
       </c>
       <c r="L215" s="6"/>
     </row>
-    <row r="216" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A216" s="4" t="s">
         <v>439</v>
       </c>
@@ -10337,7 +10316,7 @@
       </c>
       <c r="L216" s="6"/>
     </row>
-    <row r="217" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>451</v>
       </c>
@@ -10366,7 +10345,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="218" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>475</v>
       </c>
@@ -10396,7 +10375,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="219" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>476</v>
       </c>
@@ -10429,7 +10408,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="220" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>477</v>
       </c>
@@ -10465,40 +10444,40 @@
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="M142:M146">
-    <cfRule type="duplicateValues" dxfId="13" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J142:J146">
-    <cfRule type="duplicateValues" dxfId="12" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M141">
-    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M141">
-    <cfRule type="duplicateValues" dxfId="10" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J141">
-    <cfRule type="duplicateValues" dxfId="9" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K113:K117">
-    <cfRule type="duplicateValues" dxfId="8" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K118:K127">
-    <cfRule type="duplicateValues" dxfId="7" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K128:K135">
-    <cfRule type="duplicateValues" dxfId="6" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K136">
-    <cfRule type="duplicateValues" dxfId="5" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K149:K157">
-    <cfRule type="duplicateValues" dxfId="4" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K158:K162">
-    <cfRule type="duplicateValues" dxfId="2" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K179:K216">
-    <cfRule type="duplicateValues" dxfId="1" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="48"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>